<commit_message>
Finished CAstatePage. Added images. Made other minor changes.
</commit_message>
<xml_diff>
--- a/App/scraping/data/CA.xlsx
+++ b/App/scraping/data/CA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\black\Desktop\Classes\CS320\Project\Interactive_Map\App\scraping\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura\Desktop\Classes\CS320\Project\Interactive_Map\App\scraping\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215152D7-3CB4-4B7F-AD23-B4BF85C5DB03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="6510"/>
+    <workbookView xWindow="2940" yWindow="2964" windowWidth="17280" windowHeight="9348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Alcatraz Island</t>
   </si>
   <si>
-    <t>Cabrillo</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
     <t>Castle Mountains</t>
   </si>
   <si>
@@ -50,12 +45,6 @@
     <t>Golden Gate</t>
   </si>
   <si>
-    <t>Joshua Tree</t>
-  </si>
-  <si>
-    <t>Lassen Volcanic</t>
-  </si>
-  <si>
     <t>Lava Beds</t>
   </si>
   <si>
@@ -107,17 +96,46 @@
     <t>Mojave Desert</t>
   </si>
   <si>
-    <t>Juan Bautista de Anza Historic Trailhead</t>
-  </si>
-  <si>
-    <t>Channel Islands National Park</t>
+    <t>California National Historic Trail</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ésar E. Chávez National Monument</t>
+    </r>
+  </si>
+  <si>
+    <t>Channel Islands</t>
+  </si>
+  <si>
+    <t>Cabrillo National Monument</t>
+  </si>
+  <si>
+    <t>Joshua Tree National Park</t>
+  </si>
+  <si>
+    <t>Juan Bautista de Anza Historic Trail</t>
+  </si>
+  <si>
+    <t>Lassen Volcanic National Park</t>
+  </si>
+  <si>
+    <t>Yosemite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +149,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -435,161 +459,171 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>22</v>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>